<commit_message>
Add Column 'Average of Box Office Revenue' in the Pivot Table
</commit_message>
<xml_diff>
--- a/Movie_Data_Starter_Project.xlsx
+++ b/Movie_Data_Starter_Project.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20414"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Projects\Data_Analysis_Portfolio\working_with_pivot_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61F5240-81AE-4220-BA59-983E42628E40}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48AED56-A096-4BBB-861A-FC5463176592}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6536" uniqueCount="2849">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6537" uniqueCount="2850">
   <si>
     <t>Movie Title</t>
   </si>
@@ -8574,6 +8574,9 @@
   </si>
   <si>
     <t>2016</t>
+  </si>
+  <si>
+    <t>Average of Box Office Revenue ($)2</t>
   </si>
 </sst>
 </file>
@@ -8688,7 +8691,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
@@ -17286,7 +17295,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5643AB21-A11F-411C-BD6E-BF9D63A697E5}" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <location ref="A3:C9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" numFmtId="164" showAll="0">
@@ -17369,14 +17378,23 @@
       <x/>
     </i>
   </rowItems>
-  <colItems count="1">
-    <i/>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
   </colItems>
-  <dataFields count="1">
+  <dataFields count="2">
     <dataField name="Sum of Box Office Revenue ($)" fld="13" baseField="0" baseItem="0" numFmtId="44"/>
+    <dataField name="Average of Box Office Revenue ($)2" fld="13" subtotal="average" baseField="15" baseItem="2"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="4">
+    <format dxfId="6">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -17689,76 +17707,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3440AAC9-58BB-477C-9CF6-706878CD55F6}">
-  <dimension ref="A3:B9"/>
+  <dimension ref="A3:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>2841</v>
       </c>
       <c r="B3" t="s">
         <v>2843</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>2849</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
         <v>2844</v>
       </c>
       <c r="B4" s="23">
         <v>18078040000</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" s="23">
+        <v>170547547.16981131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
         <v>2845</v>
       </c>
       <c r="B5" s="23">
         <v>13672800000</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" s="23">
+        <v>160856470.58823529</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
         <v>2846</v>
       </c>
       <c r="B6" s="23">
         <v>20013420000</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" s="23">
+        <v>168180000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
         <v>2847</v>
       </c>
       <c r="B7" s="23">
         <v>13521310000</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" s="23">
+        <v>109042822.58064516</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
         <v>2848</v>
       </c>
       <c r="B8" s="23">
         <v>11921900000</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" s="23">
+        <v>161106756.75675675</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
         <v>2842</v>
       </c>
       <c r="B9" s="23">
         <v>77207470000</v>
       </c>
+      <c r="C9" s="23">
+        <v>151983208.66141734</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add column 'COUNT of Box Office Revenue'
</commit_message>
<xml_diff>
--- a/Movie_Data_Starter_Project.xlsx
+++ b/Movie_Data_Starter_Project.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20414"/>
-  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Projects\Data_Analysis_Portfolio\working_with_pivot_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48AED56-A096-4BBB-861A-FC5463176592}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5052973F-926B-40C5-8BC3-53FD7B261939}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6537" uniqueCount="2850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6538" uniqueCount="2851">
   <si>
     <t>Movie Title</t>
   </si>
@@ -8577,6 +8577,9 @@
   </si>
   <si>
     <t>Average of Box Office Revenue ($)2</t>
+  </si>
+  <si>
+    <t>Count of Box Office Revenue ($)2</t>
   </si>
 </sst>
 </file>
@@ -8691,7 +8694,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
@@ -17295,7 +17304,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5643AB21-A11F-411C-BD6E-BF9D63A697E5}" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:C9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <location ref="A3:D9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" numFmtId="164" showAll="0">
@@ -17381,20 +17390,24 @@
   <colFields count="1">
     <field x="-2"/>
   </colFields>
-  <colItems count="2">
+  <colItems count="3">
     <i>
       <x/>
     </i>
     <i i="1">
       <x v="1"/>
     </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
   </colItems>
-  <dataFields count="2">
+  <dataFields count="3">
     <dataField name="Sum of Box Office Revenue ($)" fld="13" baseField="0" baseItem="0" numFmtId="44"/>
     <dataField name="Average of Box Office Revenue ($)2" fld="13" subtotal="average" baseField="15" baseItem="2"/>
+    <dataField name="Count of Box Office Revenue ($)2" fld="13" subtotal="count" baseField="15" baseItem="2"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="6">
+    <format dxfId="8">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -17707,10 +17720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3440AAC9-58BB-477C-9CF6-706878CD55F6}">
-  <dimension ref="A3:C9"/>
+  <dimension ref="A3:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17718,9 +17731,10 @@
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>2841</v>
       </c>
@@ -17730,8 +17744,11 @@
       <c r="C3" t="s">
         <v>2849</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>2850</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
         <v>2844</v>
       </c>
@@ -17741,8 +17758,11 @@
       <c r="C4" s="23">
         <v>170547547.16981131</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" s="23">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
         <v>2845</v>
       </c>
@@ -17752,8 +17772,11 @@
       <c r="C5" s="23">
         <v>160856470.58823529</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" s="23">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
         <v>2846</v>
       </c>
@@ -17763,8 +17786,11 @@
       <c r="C6" s="23">
         <v>168180000</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" s="23">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
         <v>2847</v>
       </c>
@@ -17774,8 +17800,11 @@
       <c r="C7" s="23">
         <v>109042822.58064516</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" s="23">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
         <v>2848</v>
       </c>
@@ -17785,8 +17814,11 @@
       <c r="C8" s="23">
         <v>161106756.75675675</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" s="23">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
         <v>2842</v>
       </c>
@@ -17795,6 +17827,9 @@
       </c>
       <c r="C9" s="23">
         <v>151983208.66141734</v>
+      </c>
+      <c r="D9" s="23">
+        <v>508</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
copy paste and rename columns 2,3 and 4 of the pasted table
</commit_message>
<xml_diff>
--- a/Movie_Data_Starter_Project.xlsx
+++ b/Movie_Data_Starter_Project.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20414"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Projects\Data_Analysis_Portfolio\working_with_pivot_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5052973F-926B-40C5-8BC3-53FD7B261939}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D21F77D-E566-45B2-B572-CB17E3351DA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6538" uniqueCount="2851">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6548" uniqueCount="2854">
   <si>
     <t>Movie Title</t>
   </si>
@@ -8580,6 +8580,15 @@
   </si>
   <si>
     <t>Count of Box Office Revenue ($)2</t>
+  </si>
+  <si>
+    <t>Sum &lt; $10M</t>
+  </si>
+  <si>
+    <t>Average &lt; $10M</t>
+  </si>
+  <si>
+    <t>Count &lt; $10M</t>
   </si>
 </sst>
 </file>
@@ -8694,7 +8703,19 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="13">
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
@@ -17303,6 +17324,127 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{288B307E-74DC-482B-B13D-CC9059B04DF0}" name="PivotTable4" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A13:D19" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" numFmtId="164" showAll="0">
+      <items count="15">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="165" showAll="0"/>
+    <pivotField dataField="1" numFmtId="165" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="8">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="15"/>
+    <field x="14"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+  </colItems>
+  <dataFields count="3">
+    <dataField name="Sum &lt; $10M" fld="13" baseField="0" baseItem="0" numFmtId="44"/>
+    <dataField name="Average &lt; $10M" fld="13" subtotal="average" baseField="15" baseItem="2"/>
+    <dataField name="Count &lt; $10M" fld="13" subtotal="count" baseField="15" baseItem="2"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="3">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5643AB21-A11F-411C-BD6E-BF9D63A697E5}" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
@@ -17407,7 +17549,7 @@
     <dataField name="Count of Box Office Revenue ($)2" fld="13" subtotal="count" baseField="15" baseItem="2"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="8">
+    <format dxfId="12">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -17720,10 +17862,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3440AAC9-58BB-477C-9CF6-706878CD55F6}">
-  <dimension ref="A3:D9"/>
+  <dimension ref="A3:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17832,9 +17974,107 @@
         <v>508</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="21" t="s">
+        <v>2841</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>2851</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>2852</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>2853</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="22" t="s">
+        <v>2844</v>
+      </c>
+      <c r="B14" s="23">
+        <v>18078040000</v>
+      </c>
+      <c r="C14" s="23">
+        <v>170547547.16981131</v>
+      </c>
+      <c r="D14" s="23">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="22" t="s">
+        <v>2845</v>
+      </c>
+      <c r="B15" s="23">
+        <v>13672800000</v>
+      </c>
+      <c r="C15" s="23">
+        <v>160856470.58823529</v>
+      </c>
+      <c r="D15" s="23">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="22" t="s">
+        <v>2846</v>
+      </c>
+      <c r="B16" s="23">
+        <v>20013420000</v>
+      </c>
+      <c r="C16" s="23">
+        <v>168180000</v>
+      </c>
+      <c r="D16" s="23">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="22" t="s">
+        <v>2847</v>
+      </c>
+      <c r="B17" s="23">
+        <v>13521310000</v>
+      </c>
+      <c r="C17" s="23">
+        <v>109042822.58064516</v>
+      </c>
+      <c r="D17" s="23">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="22" t="s">
+        <v>2848</v>
+      </c>
+      <c r="B18" s="23">
+        <v>11921900000</v>
+      </c>
+      <c r="C18" s="23">
+        <v>161106756.75675675</v>
+      </c>
+      <c r="D18" s="23">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="22" t="s">
+        <v>2842</v>
+      </c>
+      <c r="B19" s="23">
+        <v>77207470000</v>
+      </c>
+      <c r="C19" s="23">
+        <v>151983208.66141734</v>
+      </c>
+      <c r="D19" s="23">
+        <v>508</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add calculated fields 'Calc Field' and 'Calc Field 1'
</commit_message>
<xml_diff>
--- a/Movie_Data_Starter_Project.xlsx
+++ b/Movie_Data_Starter_Project.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20414"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Projects\Data_Analysis_Portfolio\working_with_pivot_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D1A434-AB5A-44F8-9CCB-D2943C80BB91}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D3E1E2-5A76-4D02-A40F-3E5BF9D0F815}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,13 +21,13 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId6"/>
+    <pivotCache cacheId="31" r:id="rId6"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6550" uniqueCount="2855">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6552" uniqueCount="2857">
   <si>
     <t>Movie Title</t>
   </si>
@@ -8592,6 +8592,12 @@
   </si>
   <si>
     <t>(Multiple Items)</t>
+  </si>
+  <si>
+    <t>Calc Field</t>
+  </si>
+  <si>
+    <t>Calc Field 1</t>
   </si>
 </sst>
 </file>
@@ -8706,22 +8712,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
@@ -8766,11 +8757,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="HP" refreshedDate="45563.283721643522" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="508" xr:uid="{A8783DE5-6482-414C-806B-6CFBA141E9D9}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="HP" refreshedDate="45563.348874421295" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="508" xr:uid="{A8783DE5-6482-414C-806B-6CFBA141E9D9}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:N509" sheet="Movie Data"/>
   </cacheSource>
-  <cacheFields count="16">
+  <cacheFields count="18">
     <cacheField name="Movie Title" numFmtId="0">
       <sharedItems/>
     </cacheField>
@@ -9638,6 +9629,8 @@
         </groupItems>
       </fieldGroup>
     </cacheField>
+    <cacheField name="Calculated Field 1" numFmtId="0" formula=" SUM('Box Office Revenue ($)')/ COUNT('Box Office Revenue ($)')" databaseField="0"/>
+    <cacheField name="Calculated Field 2" numFmtId="0" formula=" SUM('Box Office Revenue ($)' )/ COUNT('Box Office Revenue ($)' )" databaseField="0"/>
   </cacheFields>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
@@ -17781,9 +17774,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{288B307E-74DC-482B-B13D-CC9059B04DF0}" name="PivotTable4" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A13:D19" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="16">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{288B307E-74DC-482B-B13D-CC9059B04DF0}" name="PivotTable4" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A13:E19" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="18">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" numFmtId="164" showAll="0">
       <items count="15">
@@ -18290,6 +18283,8 @@
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="3">
     <field x="15"/>
@@ -18319,7 +18314,7 @@
   <colFields count="1">
     <field x="-2"/>
   </colFields>
-  <colItems count="3">
+  <colItems count="4">
     <i>
       <x/>
     </i>
@@ -18329,17 +18324,21 @@
     <i i="2">
       <x v="2"/>
     </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
   </colItems>
   <pageFields count="1">
     <pageField fld="13" hier="-1"/>
   </pageFields>
-  <dataFields count="3">
+  <dataFields count="4">
     <dataField name="Sum &lt; $10M" fld="13" baseField="0" baseItem="0" numFmtId="44"/>
     <dataField name="Average &lt; $10M" fld="13" subtotal="average" baseField="15" baseItem="2"/>
     <dataField name="Count &lt; $10M" fld="13" subtotal="count" baseField="15" baseItem="2"/>
+    <dataField name="Calc Field" fld="16" baseField="15" baseItem="3" numFmtId="165"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="1">
+    <format dxfId="8">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -18356,9 +18355,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5643AB21-A11F-411C-BD6E-BF9D63A697E5}" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:D9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="16">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5643AB21-A11F-411C-BD6E-BF9D63A697E5}" name="PivotTable2" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:E9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="18">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" numFmtId="164" showAll="0">
       <items count="15">
@@ -18414,6 +18413,8 @@
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="3">
     <field x="15"/>
@@ -18443,7 +18444,7 @@
   <colFields count="1">
     <field x="-2"/>
   </colFields>
-  <colItems count="3">
+  <colItems count="4">
     <i>
       <x/>
     </i>
@@ -18453,14 +18454,18 @@
     <i i="2">
       <x v="2"/>
     </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
   </colItems>
-  <dataFields count="3">
+  <dataFields count="4">
     <dataField name="Sum of Box Office Revenue ($)" fld="13" baseField="0" baseItem="0" numFmtId="44"/>
     <dataField name="Average of Box Office Revenue ($)2" fld="13" subtotal="average" baseField="15" baseItem="2"/>
     <dataField name="Count of Box Office Revenue ($)2" fld="13" subtotal="count" baseField="15" baseItem="2"/>
+    <dataField name="Calc Field 1" fld="17" baseField="15" baseItem="1" numFmtId="165"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="14">
+    <format dxfId="9">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -18773,21 +18778,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3440AAC9-58BB-477C-9CF6-706878CD55F6}">
-  <dimension ref="A3:D19"/>
+  <dimension ref="A3:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="23" width="14" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="15" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15" bestFit="1" customWidth="1"/>
+    <col min="28" max="33" width="14" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="15" bestFit="1" customWidth="1"/>
+    <col min="37" max="42" width="14" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="83" width="14" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="85" max="124" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="125" max="146" width="14" bestFit="1" customWidth="1"/>
+    <col min="147" max="148" width="15" bestFit="1" customWidth="1"/>
+    <col min="149" max="149" width="14" bestFit="1" customWidth="1"/>
+    <col min="150" max="150" width="15" bestFit="1" customWidth="1"/>
+    <col min="151" max="156" width="14" bestFit="1" customWidth="1"/>
+    <col min="157" max="159" width="15" bestFit="1" customWidth="1"/>
+    <col min="160" max="165" width="14" bestFit="1" customWidth="1"/>
+    <col min="166" max="166" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="167" max="167" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="168" max="168" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="169" max="169" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>2841</v>
       </c>
@@ -18800,8 +18829,11 @@
       <c r="D3" t="s">
         <v>2850</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>2856</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
         <v>2844</v>
       </c>
@@ -18814,8 +18846,11 @@
       <c r="D4" s="23">
         <v>106</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="23">
+        <v>18078040000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
         <v>2845</v>
       </c>
@@ -18828,8 +18863,11 @@
       <c r="D5" s="23">
         <v>85</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="23">
+        <v>13672800000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
         <v>2846</v>
       </c>
@@ -18842,8 +18880,11 @@
       <c r="D6" s="23">
         <v>119</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="23">
+        <v>20013420000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
         <v>2847</v>
       </c>
@@ -18856,8 +18897,11 @@
       <c r="D7" s="23">
         <v>124</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="23">
+        <v>13521310000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
         <v>2848</v>
       </c>
@@ -18870,8 +18914,11 @@
       <c r="D8" s="23">
         <v>74</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" s="23">
+        <v>11921900000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
         <v>2842</v>
       </c>
@@ -18884,8 +18931,11 @@
       <c r="D9" s="23">
         <v>508</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" s="23">
+        <v>77207470000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
         <v>13</v>
       </c>
@@ -18893,7 +18943,7 @@
         <v>2854</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="21" t="s">
         <v>2841</v>
       </c>
@@ -18906,8 +18956,11 @@
       <c r="D13" t="s">
         <v>2853</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>2855</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="22" t="s">
         <v>2844</v>
       </c>
@@ -18920,8 +18973,11 @@
       <c r="D14" s="23">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" s="23">
+        <v>67940000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="22" t="s">
         <v>2845</v>
       </c>
@@ -18934,8 +18990,11 @@
       <c r="D15" s="23">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" s="23">
+        <v>26400000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
         <v>2846</v>
       </c>
@@ -18948,8 +19007,11 @@
       <c r="D16" s="23">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="23">
+        <v>46920000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="22" t="s">
         <v>2847</v>
       </c>
@@ -18962,8 +19024,11 @@
       <c r="D17" s="23">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="23">
+        <v>93040000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="22" t="s">
         <v>2848</v>
       </c>
@@ -18976,8 +19041,11 @@
       <c r="D18" s="23">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="23">
+        <v>41100000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
         <v>2842</v>
       </c>
@@ -18989,6 +19057,9 @@
       </c>
       <c r="D19" s="23">
         <v>57</v>
+      </c>
+      <c r="E19" s="23">
+        <v>275400000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add 'Percent of total movies' column
</commit_message>
<xml_diff>
--- a/Movie_Data_Starter_Project.xlsx
+++ b/Movie_Data_Starter_Project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Projects\Data_Analysis_Portfolio\working_with_pivot_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D3E1E2-5A76-4D02-A40F-3E5BF9D0F815}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CDA84B-08C8-4AC5-AE67-F93F27C214FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Directors" sheetId="3" r:id="rId4"/>
     <sheet name="Actors" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="31" r:id="rId6"/>
   </pivotCaches>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6552" uniqueCount="2857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6553" uniqueCount="2858">
   <si>
     <t>Movie Title</t>
   </si>
@@ -8598,6 +8598,9 @@
   </si>
   <si>
     <t>Calc Field 1</t>
+  </si>
+  <si>
+    <t>Percent of total movies</t>
   </si>
 </sst>
 </file>
@@ -8609,7 +8612,7 @@
     <numFmt numFmtId="164" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -8633,6 +8636,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -8658,10 +8668,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -8708,9 +8719,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -18778,10 +18793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3440AAC9-58BB-477C-9CF6-706878CD55F6}">
-  <dimension ref="A3:E19"/>
+  <dimension ref="A3:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18792,7 +18807,8 @@
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="23" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="23" width="14" bestFit="1" customWidth="1"/>
     <col min="24" max="25" width="15" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="14" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="15" bestFit="1" customWidth="1"/>
@@ -18816,7 +18832,7 @@
     <col min="169" max="169" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>2841</v>
       </c>
@@ -18833,7 +18849,7 @@
         <v>2856</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
         <v>2844</v>
       </c>
@@ -18850,7 +18866,7 @@
         <v>18078040000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
         <v>2845</v>
       </c>
@@ -18867,7 +18883,7 @@
         <v>13672800000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
         <v>2846</v>
       </c>
@@ -18884,7 +18900,7 @@
         <v>20013420000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
         <v>2847</v>
       </c>
@@ -18901,7 +18917,7 @@
         <v>13521310000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
         <v>2848</v>
       </c>
@@ -18918,7 +18934,7 @@
         <v>11921900000</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
         <v>2842</v>
       </c>
@@ -18935,7 +18951,7 @@
         <v>77207470000</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
         <v>13</v>
       </c>
@@ -18943,7 +18959,7 @@
         <v>2854</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="21" t="s">
         <v>2841</v>
       </c>
@@ -18959,8 +18975,11 @@
       <c r="E13" t="s">
         <v>2855</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G13" s="24" t="s">
+        <v>2857</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="22" t="s">
         <v>2844</v>
       </c>
@@ -18976,8 +18995,12 @@
       <c r="E14" s="23">
         <v>67940000</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G14" s="26">
+        <f>D14/D4</f>
+        <v>9.4339622641509441E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="22" t="s">
         <v>2845</v>
       </c>
@@ -18993,8 +19016,12 @@
       <c r="E15" s="23">
         <v>26400000</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G15" s="26">
+        <f t="shared" ref="G15:G19" si="0">D15/D5</f>
+        <v>9.4117647058823528E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
         <v>2846</v>
       </c>
@@ -19010,8 +19037,12 @@
       <c r="E16" s="23">
         <v>46920000</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G16" s="26">
+        <f t="shared" si="0"/>
+        <v>9.2436974789915971E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="22" t="s">
         <v>2847</v>
       </c>
@@ -19027,8 +19058,12 @@
       <c r="E17" s="23">
         <v>93040000</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G17" s="26">
+        <f t="shared" si="0"/>
+        <v>0.16129032258064516</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="22" t="s">
         <v>2848</v>
       </c>
@@ -19044,8 +19079,12 @@
       <c r="E18" s="23">
         <v>41100000</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G18" s="26">
+        <f t="shared" si="0"/>
+        <v>0.10810810810810811</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
         <v>2842</v>
       </c>
@@ -19061,6 +19100,7 @@
       <c r="E19" s="23">
         <v>275400000</v>
       </c>
+      <c r="G19" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>